<commit_message>
slight changes to 05.22 CVM results for demo purposes
</commit_message>
<xml_diff>
--- a/Archive/JSON/2024-05-22/2024-05-22_CVMResults.xlsx
+++ b/Archive/JSON/2024-05-22/2024-05-22_CVMResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nventco-my.sharepoint.com/personal/e1176752_nventco_com/Documents/Documents/VSCode/Projects/LPSD/LPSD/Archive/JSON/2024-05-22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_23FA9B513A25D79E2B002F7AFBBDA7149C65DFBF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{554829C2-4B35-4308-884F-AB797AC489EC}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_23FA9B513A25D79E2B002F7AFBBDA7149C65DFBF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E212E44-7348-4FE1-92B4-39061842117B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="6" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28956,11 +28956,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -33407,8 +33410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q95"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:P94"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="M100" sqref="M100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>